<commit_message>
Moved class. Stream, FunctionalInterface
</commit_message>
<xml_diff>
--- a/Next.xlsx
+++ b/Next.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDrive\GitHub\cognitiveLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD5D621-63C1-4CDA-906B-569D530A8266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC953B39-5025-4CBC-BFD1-64B4D8681E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="whatIs" sheetId="1" r:id="rId1"/>
-    <sheet name="Thread" sheetId="3" r:id="rId2"/>
-    <sheet name="Learn" sheetId="2" r:id="rId3"/>
+    <sheet name="Learn" sheetId="2" r:id="rId2"/>
+    <sheet name="Thread" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="86">
   <si>
     <t>Enivromnent</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>ReEntrantLock</t>
+  </si>
+  <si>
+    <t>Executor Interface</t>
   </si>
 </sst>
 </file>
@@ -775,7 +778,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1087,11 +1090,120 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72B8DA3-A3FB-4C46-AA4C-783C6BE00117}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="9"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="9"/>
+    </row>
+    <row r="5" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EB39DF-7615-411B-98EB-4C67F06EA483}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1231,117 +1343,13 @@
         <v>84</v>
       </c>
     </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C29" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72B8DA3-A3FB-4C46-AA4C-783C6BE00117}">
-  <dimension ref="A1:B25"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="18.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="9"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="9"/>
-    </row>
-    <row r="5" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="9"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="9"/>
-    </row>
-    <row r="9" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>